<commit_message>
trust, distance payments, double spending, async payments
</commit_message>
<xml_diff>
--- a/Research/target_analysis.xlsx
+++ b/Research/target_analysis.xlsx
@@ -238,7 +238,7 @@
     <t xml:space="preserve">https://www.gsma.com/mobilefordevelopment/wp-content/uploads/2018/09/State-of-Mobile-Internet-Connectivity-2018.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Data affordability (100mb) 
+    <t xml:space="preserve">Data affordability (100MB) 
 (of monthly GDP per capita)</t>
   </si>
   <si>
@@ -434,6 +434,7 @@
         <sz val="13"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">List of countries where mobile money has been a success / failure
 </t>
@@ -443,6 +444,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">http://www.ijbmi.org/papers/Vol(6)4/G06047887.pdf</t>
     </r>
@@ -457,6 +459,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Failed in</t>
     </r>
@@ -465,6 +468,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">: Burkina Faso, Ghana, Haiti, India, Indonesia, Madagascar</t>
     </r>
@@ -476,6 +480,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Weak growth: </t>
     </r>
@@ -484,6 +489,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pakistan, Philipines</t>
     </r>
@@ -495,6 +501,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">High growth: </t>
     </r>
@@ -503,6 +510,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Bangladesh, Côte d'Ivoire, Kenya, Rwanda, Somaliland, Tanzania, Uganda, Zimbawbe</t>
     </r>
@@ -551,6 +559,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Need to have
 </t>
@@ -560,6 +569,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Focus on Africa, parts of Asia or parts of Latin America
 - Focus on a non-internet-based solution to cover rural areas and take the gap between cellular devices and internet into account
@@ -573,6 +583,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Nice to have
 </t>
@@ -582,6 +593,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Cheap such that those who cite lack of money and expensive bank accounts are allowed to board the system
 - Without identification to enable those without a valid ID
@@ -603,6 +615,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -624,24 +637,28 @@
       <sz val="15"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -738,12 +755,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -835,18 +852,26 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -891,23 +916,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -994,11 +1023,11 @@
   </sheetPr>
   <dimension ref="A1:BM71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.3"/>
@@ -1006,7 +1035,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="114.79"/>
@@ -1416,77 +1445,77 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="36"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
     </row>
     <row r="24" customFormat="false" ht="147" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
@@ -1495,7 +1524,7 @@
       <c r="C24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="39" t="s">
         <v>98</v>
       </c>
       <c r="E24" s="24" t="s">
@@ -1503,7 +1532,7 @@
       </c>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="28" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1517,11 +1546,11 @@
       <c r="D25" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
@@ -1533,11 +1562,11 @@
       <c r="D26" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
@@ -1549,38 +1578,38 @@
       <c r="D27" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
     </row>
     <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="4" t="s">
@@ -1588,25 +1617,25 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="4" t="s">
@@ -1617,17 +1646,17 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="G42" s="41" t="s">
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="G42" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
@@ -1643,17 +1672,17 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="42" t="s">
+      <c r="B48" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="F48" s="42" t="s">
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="F48" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="23" t="s">
@@ -1661,210 +1690,210 @@
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="23"/>
-      <c r="F49" s="43" t="s">
+      <c r="F49" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
       <c r="D50" s="23"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
       <c r="D51" s="23"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
       <c r="D52" s="23"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
       <c r="D53" s="23"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
       <c r="D54" s="23"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
       <c r="D55" s="23"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
       <c r="D56" s="23"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="23"/>
       <c r="C57" s="23"/>
       <c r="D57" s="23"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
       <c r="D58" s="23"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
       <c r="D59" s="23"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
       <c r="D60" s="23"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
       <c r="D61" s="23"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
       <c r="D62" s="23"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
       <c r="D63" s="23"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
       <c r="D64" s="23"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
       <c r="D65" s="23"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
       <c r="D66" s="23"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="23"/>
       <c r="C67" s="23"/>
       <c r="D67" s="23"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
       <c r="D68" s="23"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
       <c r="D69" s="23"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="46"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="23"/>
       <c r="C70" s="23"/>
       <c r="D70" s="23"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
       <c r="D71" s="23"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="46"/>
+      <c r="I71" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>